<commit_message>
renaming EWS to ESS
</commit_message>
<xml_diff>
--- a/data/scenarios.xlsx
+++ b/data/scenarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB854A84-F65C-5645-9B14-2B6ACE59A967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB1CACD-C21E-0348-8641-790887F3344C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" xr2:uid="{2F6A880A-CADF-8941-BACA-B4A1F43DB678}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="44">
   <si>
     <t>Scenario</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>Base-case</t>
+  </si>
+  <si>
+    <t>NPIs w/o ESS</t>
+  </si>
+  <si>
+    <t>NPIs + 2-day ESS</t>
+  </si>
+  <si>
+    <t>NPIs + 5-day ESS</t>
+  </si>
+  <si>
+    <t>NPIs + 10-day ESS</t>
   </si>
 </sst>
 </file>
@@ -643,7 +655,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F2" s="5">
         <f>[1]parameters!$D$22</f>
@@ -819,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="F4" s="5">
         <f>F$2</f>
@@ -871,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="F5" s="5">
         <f>F$2</f>
@@ -923,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="F6" s="5">
         <f>F$2</f>

</xml_diff>